<commit_message>
#76 #73 #78 #74 #72 #75
</commit_message>
<xml_diff>
--- a/Docs/Testing (TES)/TS_home_menu_recent_logo_head_foot.xlsx
+++ b/Docs/Testing (TES)/TS_home_menu_recent_logo_head_foot.xlsx
@@ -63,9 +63,6 @@
     <t>Убедиться, что после нажатия кнопки войти, мы перешли на страницу http://www.vashchenko.ru/admin-room</t>
   </si>
   <si>
-    <t>Дополнительные условия, выполняемые перед каждым тестом</t>
-  </si>
-  <si>
     <t>TS_home_001</t>
   </si>
   <si>
@@ -379,6 +376,9 @@
   </si>
   <si>
     <t>http://www.vashchenko.ru/albums/&lt;название альбома&gt;/&lt;номер страницы&gt;</t>
+  </si>
+  <si>
+    <t>Дополнительные условия</t>
   </si>
 </sst>
 </file>
@@ -490,13 +490,13 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1014,8 +1014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1053,19 +1053,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="D2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="F2" s="11" t="s">
         <v>19</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1073,19 +1073,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="D3" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="E3" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="F3" s="11" t="s">
         <v>24</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1093,19 +1093,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="D4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="E4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="11" t="s">
         <v>28</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -1113,19 +1113,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="D5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="13" t="s">
+      <c r="F5" s="14" t="s">
         <v>32</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -1133,19 +1133,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="14" t="s">
         <v>34</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -1153,39 +1153,39 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="13" t="s">
+      <c r="F7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:6" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="14" t="s">
         <v>39</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -1193,19 +1193,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="D9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="11" t="s">
         <v>42</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -1213,19 +1213,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="11" t="s">
         <v>44</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1233,19 +1233,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="D11" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="11" t="s">
         <v>47</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1253,19 +1253,19 @@
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="D12" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="11" t="s">
         <v>50</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -1273,19 +1273,19 @@
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="D13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="11" t="s">
         <v>53</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -1293,19 +1293,19 @@
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" s="11" t="s">
         <v>55</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -1313,19 +1313,19 @@
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" s="14" t="s">
         <v>57</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -1333,19 +1333,19 @@
         <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16" s="14" t="s">
         <v>59</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1353,19 +1353,19 @@
         <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="D17" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="E17" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="F17" s="11" t="s">
         <v>64</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -1373,17 +1373,17 @@
         <v>17</v>
       </c>
       <c r="B18" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>67</v>
-      </c>
       <c r="D18" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E18" s="10"/>
       <c r="F18" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -1391,19 +1391,19 @@
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="D19" t="s">
         <v>70</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="9" t="s">
         <v>71</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -1411,19 +1411,19 @@
         <v>19</v>
       </c>
       <c r="B20" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="D20" t="s">
+        <v>70</v>
+      </c>
+      <c r="E20" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="D20" t="s">
-        <v>71</v>
-      </c>
-      <c r="E20" s="15" t="s">
+      <c r="F20" s="8" t="s">
         <v>75</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="105" x14ac:dyDescent="0.25">
@@ -1431,19 +1431,19 @@
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C21" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="D21" t="s">
+        <v>70</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F21" s="8" t="s">
         <v>78</v>
-      </c>
-      <c r="D21" t="s">
-        <v>71</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1451,19 +1451,19 @@
         <v>21</v>
       </c>
       <c r="B22" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="D22" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="F22" s="9" t="s">
         <v>81</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="120" x14ac:dyDescent="0.25">
@@ -1471,19 +1471,19 @@
         <v>22</v>
       </c>
       <c r="B23" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C23" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="D23" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="8" t="s">
         <v>84</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="120" x14ac:dyDescent="0.25">
@@ -1491,19 +1491,19 @@
         <v>23</v>
       </c>
       <c r="B24" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" s="8" t="s">
         <v>86</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1511,17 +1511,17 @@
         <v>24</v>
       </c>
       <c r="B25" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="D25" s="6" t="s">
         <v>89</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>90</v>
       </c>
       <c r="E25" s="10"/>
       <c r="F25" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1542,7 +1542,7 @@
     </row>
     <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>15</v>
+        <v>120</v>
       </c>
       <c r="D29" s="5"/>
       <c r="F29" s="8"/>
@@ -1555,7 +1555,7 @@
     </row>
     <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D31" s="5"/>
     </row>
@@ -1572,7 +1572,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1600,131 +1600,131 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
+        <v>94</v>
+      </c>
+      <c r="C38" s="6" t="s">
         <v>95</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>10</v>
       </c>
-      <c r="C39" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="D39" s="21"/>
+      <c r="C39" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="D39" s="22"/>
     </row>
     <row r="40" spans="1:4" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
+        <v>97</v>
+      </c>
+      <c r="C40" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="C40" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="D40" s="21"/>
+      <c r="D40" s="22"/>
     </row>
     <row r="41" spans="1:4" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
+        <v>99</v>
+      </c>
+      <c r="C41" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="C41" s="22" t="s">
-        <v>101</v>
-      </c>
-      <c r="D41" s="22"/>
+      <c r="D41" s="23"/>
     </row>
     <row r="42" spans="1:4" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
+        <v>101</v>
+      </c>
+      <c r="C42" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="C42" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="D42" s="21"/>
+      <c r="D42" s="22"/>
     </row>
     <row r="43" spans="1:4" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
+        <v>103</v>
+      </c>
+      <c r="C43" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="C43" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="D43" s="21"/>
+      <c r="D43" s="22"/>
     </row>
     <row r="44" spans="1:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
+        <v>105</v>
+      </c>
+      <c r="C44" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="C44" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="D44" s="21"/>
+      <c r="D44" s="22"/>
     </row>
     <row r="45" spans="1:4" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
+        <v>107</v>
+      </c>
+      <c r="C45" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="C45" s="21" t="s">
-        <v>109</v>
-      </c>
-      <c r="D45" s="21"/>
+      <c r="D45" s="22"/>
     </row>
     <row r="46" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
+        <v>109</v>
+      </c>
+      <c r="C46" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="C46" s="21" t="s">
-        <v>111</v>
-      </c>
-      <c r="D46" s="21"/>
+      <c r="D46" s="22"/>
     </row>
     <row r="47" spans="1:4" ht="174.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>82</v>
-      </c>
-      <c r="C47" s="23" t="s">
-        <v>112</v>
-      </c>
-      <c r="D47" s="23"/>
+        <v>81</v>
+      </c>
+      <c r="C47" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="D47" s="21"/>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C72" s="19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C73" s="19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C74" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C75" s="20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C76" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>